<commit_message>
update the code with newer version
</commit_message>
<xml_diff>
--- a/AgentProxy/jobdata.xlsx
+++ b/AgentProxy/jobdata.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\BTP2_new\apidev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\MAS-GUI\AgentProxy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14850" windowHeight="5985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14850" windowHeight="5985" activeTab="9"/>
   </bookViews>
   <sheets>
-    <sheet name="job1" sheetId="1" r:id="rId1"/>
+    <sheet name="job1" sheetId="11" r:id="rId1"/>
     <sheet name="job2" sheetId="2" r:id="rId2"/>
     <sheet name="job3" sheetId="3" r:id="rId3"/>
     <sheet name="job4" sheetId="4" r:id="rId4"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Attributes</t>
-  </si>
-  <si>
-    <t>10,23</t>
   </si>
   <si>
     <t>A2</t>
@@ -66,19 +63,16 @@
     <t>Processing Times</t>
   </si>
   <si>
-    <t>operation1</t>
+    <t>Penalty Rate</t>
   </si>
   <si>
-    <t>Penalty</t>
+    <t>Operation_1</t>
   </si>
   <si>
-    <t>operation2</t>
+    <t>Operation_2</t>
   </si>
   <si>
-    <t>9,12</t>
-  </si>
-  <si>
-    <t>operation3</t>
+    <t>Operation_3</t>
   </si>
 </sst>
 </file>
@@ -568,9 +562,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="33" borderId="3" xfId="4" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -631,7 +624,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D6" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Table126" displayName="Table126" ref="A1:D6" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
   <autoFilter ref="A1:D6"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
@@ -647,7 +640,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table312" displayName="Table312" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -670,7 +663,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table314" displayName="Table314" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -693,7 +686,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table316" displayName="Table316" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -716,7 +709,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table318" displayName="Table318" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -739,7 +732,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table320" displayName="Table320" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -759,10 +752,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="E1:E2" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Table327" displayName="Table327" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -772,7 +765,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table322" displayName="Table322" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -795,7 +788,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -818,7 +811,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table38" displayName="Table38" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -841,7 +834,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table310" displayName="Table310" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1123,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1128,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1146,13 +1139,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1169,20 +1162,20 @@
         <v>10</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1193,30 +1186,30 @@
       <c r="B4">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
+      <c r="C5">
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -1225,17 +1218,8 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E10" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="1"/>
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1250,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,7 +1244,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1271,13 +1255,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1294,20 +1278,20 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1318,30 +1302,30 @@
       <c r="B4">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
+      <c r="C5">
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -1350,7 +1334,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1367,7 +1351,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,7 +1360,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1387,13 +1371,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1410,20 +1394,20 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1434,16 +1418,16 @@
       <c r="B4">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>9</v>
@@ -1452,7 +1436,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1469,7 +1453,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,7 +1462,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1489,13 +1473,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1516,16 +1500,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1536,11 +1520,11 @@
       <c r="B4">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1557,7 +1541,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,7 +1550,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1577,13 +1561,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1604,16 +1588,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1624,25 +1608,25 @@
       <c r="B4">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
+      <c r="C5">
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1659,7 +1643,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D16:D17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,7 +1652,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1679,13 +1663,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1702,20 +1686,20 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1726,30 +1710,30 @@
       <c r="B4">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
+      <c r="C5">
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -1758,7 +1742,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1775,7 +1759,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1784,7 +1768,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1795,13 +1779,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1822,16 +1806,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1842,25 +1826,25 @@
       <c r="B4">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
+      <c r="C5">
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1877,7 +1861,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1886,7 +1870,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1897,13 +1881,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1920,35 +1904,35 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1965,7 +1949,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1974,7 +1958,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1985,13 +1969,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2012,16 +1996,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2032,30 +2016,30 @@
       <c r="B4">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
+      <c r="C5">
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -2064,7 +2048,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2081,7 +2065,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2090,7 +2074,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2101,13 +2085,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2124,49 +2108,49 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
+      <c r="C5">
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mend table column size of all tables *** update the job file *** change jobloader for new job file *** update GUI for operations of job
</commit_message>
<xml_diff>
--- a/AgentProxy/jobdata.xlsx
+++ b/AgentProxy/jobdata.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="52">
   <si>
     <t>id</t>
   </si>
@@ -36,43 +36,154 @@
     <t>quantity</t>
   </si>
   <si>
-    <t>Dimensions</t>
-  </si>
-  <si>
-    <t>Attributes</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
     <t>CPN</t>
   </si>
   <si>
     <t>Due Date (Seconds)</t>
   </si>
   <si>
-    <t>Operation Type</t>
-  </si>
-  <si>
-    <t>Processing Times</t>
-  </si>
-  <si>
     <t>Penalty Rate</t>
   </si>
   <si>
-    <t>Operation_1</t>
-  </si>
-  <si>
-    <t>Operation_2</t>
-  </si>
-  <si>
-    <t>Operation_3</t>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>j1</t>
+  </si>
+  <si>
+    <t>j2</t>
+  </si>
+  <si>
+    <t>j3</t>
+  </si>
+  <si>
+    <t>j4</t>
+  </si>
+  <si>
+    <t>j6</t>
+  </si>
+  <si>
+    <t>j5</t>
+  </si>
+  <si>
+    <t>j7</t>
+  </si>
+  <si>
+    <t>j8</t>
+  </si>
+  <si>
+    <t>j9</t>
+  </si>
+  <si>
+    <t>j10</t>
+  </si>
+  <si>
+    <t>j1o1</t>
+  </si>
+  <si>
+    <t>j1o2</t>
+  </si>
+  <si>
+    <t>j1o3</t>
+  </si>
+  <si>
+    <t>j2o1</t>
+  </si>
+  <si>
+    <t>j2o2</t>
+  </si>
+  <si>
+    <t>j2o3</t>
+  </si>
+  <si>
+    <t>j2o4</t>
+  </si>
+  <si>
+    <t>j2o5</t>
+  </si>
+  <si>
+    <t>j3o1</t>
+  </si>
+  <si>
+    <t>j4o1</t>
+  </si>
+  <si>
+    <t>j4o2</t>
+  </si>
+  <si>
+    <t>j5o1</t>
+  </si>
+  <si>
+    <t>j6o1</t>
+  </si>
+  <si>
+    <t>j6o2</t>
+  </si>
+  <si>
+    <t>j6o3</t>
+  </si>
+  <si>
+    <t>j6o4</t>
+  </si>
+  <si>
+    <t>j7o1</t>
+  </si>
+  <si>
+    <t>j7o2</t>
+  </si>
+  <si>
+    <t>j7o3</t>
+  </si>
+  <si>
+    <t>j7o4</t>
+  </si>
+  <si>
+    <t>j7o5</t>
+  </si>
+  <si>
+    <t>j7o6</t>
+  </si>
+  <si>
+    <t>j8o1</t>
+  </si>
+  <si>
+    <t>j8o2</t>
+  </si>
+  <si>
+    <t>j9o1</t>
+  </si>
+  <si>
+    <t>j9o2</t>
+  </si>
+  <si>
+    <t>j9o3</t>
+  </si>
+  <si>
+    <t>j9o4</t>
+  </si>
+  <si>
+    <t>j10o1</t>
+  </si>
+  <si>
+    <t>j10o2</t>
+  </si>
+  <si>
+    <t>j10o3</t>
+  </si>
+  <si>
+    <t>j10o4</t>
+  </si>
+  <si>
+    <t>j10o5</t>
+  </si>
+  <si>
+    <t>j10o6</t>
+  </si>
+  <si>
+    <t>j10o7</t>
+  </si>
+  <si>
+    <t>j10o8</t>
   </si>
 </sst>
 </file>
@@ -397,7 +508,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -564,7 +675,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="3" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -624,8 +735,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Table126" displayName="Table126" ref="A1:D6" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
-  <autoFilter ref="A1:D6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Table126" displayName="Table126" ref="A1:D2" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
+  <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="3" name="quantity"/>
@@ -647,8 +758,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table113" displayName="Table113" ref="A1:D5" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
-  <autoFilter ref="A1:D5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table113" displayName="Table113" ref="A1:D2" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
+  <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="3" name="quantity"/>
@@ -670,8 +781,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table115" displayName="Table115" ref="A1:D4" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
-  <autoFilter ref="A1:D4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table115" displayName="Table115" ref="A1:D2" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
+  <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="3" name="quantity"/>
@@ -693,8 +804,8 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table117" displayName="Table117" ref="A1:D6" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
-  <autoFilter ref="A1:D6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table117" displayName="Table117" ref="A1:D2" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
+  <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="3" name="quantity"/>
@@ -716,8 +827,8 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table119" displayName="Table119" ref="A1:D5" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
-  <autoFilter ref="A1:D5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table119" displayName="Table119" ref="A1:D2" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
+  <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="3" name="quantity"/>
@@ -739,8 +850,8 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table121" displayName="Table121" ref="A1:D6" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
-  <autoFilter ref="A1:D6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table121" displayName="Table121" ref="A1:D2" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
+  <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="3" name="quantity"/>
@@ -772,8 +883,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:D5" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
-  <autoFilter ref="A1:D5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:D2" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
+  <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="3" name="quantity"/>
@@ -795,8 +906,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table17" displayName="Table17" ref="A1:D4" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
-  <autoFilter ref="A1:D4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table17" displayName="Table17" ref="A1:D2" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
+  <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="3" name="quantity"/>
@@ -818,8 +929,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table19" displayName="Table19" ref="A1:D5" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
-  <autoFilter ref="A1:D5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table19" displayName="Table19" ref="A1:D2" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
+  <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="3" name="quantity"/>
@@ -841,8 +952,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table111" displayName="Table111" ref="A1:D6" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
-  <autoFilter ref="A1:D6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table111" displayName="Table111" ref="A1:D2" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
+  <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="3" name="quantity"/>
@@ -1119,7 +1230,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,18 +1250,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11</v>
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -1165,60 +1276,24 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>13</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1232,10 +1307,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,18 +1330,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1010</v>
+      <c r="A2" t="s">
+        <v>15</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -1281,60 +1356,49 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1348,10 +1412,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,18 +1435,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>22</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -1397,46 +1461,34 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1453,7 +1505,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,18 +1525,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>33</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -1499,32 +1551,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1541,7 +1575,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,18 +1595,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>44</v>
+      <c r="A2" t="s">
+        <v>9</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -1587,46 +1621,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1640,10 +1647,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1663,18 +1670,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>55</v>
       </c>
       <c r="B2">
         <v>7</v>
@@ -1689,60 +1696,14 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1756,10 +1717,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,18 +1740,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>66</v>
+      <c r="A2" t="s">
+        <v>10</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -1805,46 +1766,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5">
-        <v>21</v>
-      </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1858,10 +1802,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1881,18 +1825,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>77</v>
+      <c r="A2" t="s">
+        <v>12</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -1907,32 +1851,39 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1946,10 +1897,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1969,18 +1920,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>88</v>
+      <c r="A2" t="s">
+        <v>13</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -1995,60 +1946,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>21</v>
-      </c>
-      <c r="C4">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2062,10 +1972,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2085,18 +1995,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>99</v>
+      <c r="A2" t="s">
+        <v>14</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -2111,46 +2021,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>17</v>
-      </c>
-      <c r="C5">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>